<commit_message>
Update Storage goose list
</commit_message>
<xml_diff>
--- a/研发仓库物料清单.xlsx
+++ b/研发仓库物料清单.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="215">
   <si>
     <t>名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -320,10 +320,6 @@
   </si>
   <si>
     <t>主机</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>抬</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -820,6 +816,71 @@
   </si>
   <si>
     <t>使用登记</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>风扇平台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP_008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018.12.11 机电部
+刘杰、黄涛放入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8个风扇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018.12.4日张禄禄、
+王欢放入一个主机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连接线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShY_012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018.12.4日张禄禄、
+王欢放入一箱连接线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShY_011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018.12.4日张禄禄、
+王欢放入一箱显示器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018.12.4日张禄禄、
+王欢放入一个A5探测器包装箱</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -887,7 +948,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -934,6 +995,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1240,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA86"/>
+  <dimension ref="A1:AA89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:Z1"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1255,7 +1323,7 @@
     <col min="5" max="5" width="9.375" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.25" customWidth="1"/>
     <col min="7" max="7" width="14.625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="18.25" customWidth="1"/>
+    <col min="8" max="8" width="22.25" customWidth="1"/>
     <col min="9" max="9" width="17.625" customWidth="1"/>
     <col min="10" max="10" width="17.75" customWidth="1"/>
   </cols>
@@ -1265,7 +1333,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1280,10 +1348,10 @@
         <v>2</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
@@ -1306,7 +1374,7 @@
       <c r="AA1" s="3"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="1">
@@ -1322,11 +1390,11 @@
         <v>7</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A3" s="18"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="1">
         <v>2</v>
       </c>
@@ -1340,19 +1408,19 @@
         <v>17</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="1">
@@ -1368,11 +1436,11 @@
         <v>22</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A6" s="18"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1389,11 +1457,11 @@
         <v>24</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A7" s="18"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1410,11 +1478,11 @@
         <v>24</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A8" s="18"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -1428,11 +1496,11 @@
         <v>22</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A9" s="18"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="1">
         <v>5</v>
       </c>
@@ -1446,11 +1514,11 @@
         <v>22</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A10" s="18"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="1">
         <v>6</v>
       </c>
@@ -1464,11 +1532,11 @@
         <v>23</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A11" s="18"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="1">
         <v>7</v>
       </c>
@@ -1482,11 +1550,11 @@
         <v>23</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A12" s="18"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="1">
         <v>8</v>
       </c>
@@ -1500,11 +1568,11 @@
         <v>23</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A13" s="18"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="1">
         <v>9</v>
       </c>
@@ -1518,11 +1586,11 @@
         <v>23</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A14" s="18"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="1">
         <v>10</v>
       </c>
@@ -1536,11 +1604,11 @@
         <v>33</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A15" s="18"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="1">
         <v>11</v>
       </c>
@@ -1554,11 +1622,11 @@
         <v>35</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A16" s="18"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="1">
         <v>12</v>
       </c>
@@ -1572,11 +1640,11 @@
         <v>22</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17" s="18"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A17" s="21"/>
       <c r="B17" s="1">
         <v>13</v>
       </c>
@@ -1590,11 +1658,11 @@
         <v>35</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18" s="18"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18" s="21"/>
       <c r="B18" s="1">
         <v>14</v>
       </c>
@@ -1605,22 +1673,22 @@
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F18" t="s">
         <v>198</v>
       </c>
-      <c r="F18" t="s">
-        <v>199</v>
-      </c>
       <c r="G18" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="18"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="21"/>
       <c r="B19" s="7">
         <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D19" s="10">
         <v>2</v>
@@ -1629,19 +1697,19 @@
         <v>12</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A21" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="1">
@@ -1657,11 +1725,11 @@
         <v>7</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="18"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A22" s="21"/>
       <c r="B22" s="1">
         <v>2</v>
       </c>
@@ -1675,11 +1743,11 @@
         <v>7</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="18"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A23" s="21"/>
       <c r="B23" s="1">
         <v>3</v>
       </c>
@@ -1693,11 +1761,11 @@
         <v>7</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="18"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A24" s="21"/>
       <c r="B24" s="1">
         <v>4</v>
       </c>
@@ -1711,11 +1779,11 @@
         <v>7</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="18"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A25" s="21"/>
       <c r="B25" s="1">
         <v>5</v>
       </c>
@@ -1729,11 +1797,11 @@
         <v>12</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" s="18"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A26" s="21"/>
       <c r="B26" s="1">
         <v>6</v>
       </c>
@@ -1747,11 +1815,11 @@
         <v>7</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" s="18"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A27" s="21"/>
       <c r="B27" s="1">
         <v>7</v>
       </c>
@@ -1765,559 +1833,564 @@
         <v>7</v>
       </c>
       <c r="G27" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="17" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A28" s="21"/>
+      <c r="B28" s="18">
+        <v>8</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="D28" s="18">
+        <v>1</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A30" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="10">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A29" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="10">
-        <v>1</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G29" s="10" t="s">
+    <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="21"/>
+      <c r="B31" s="10">
+        <v>2</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D31" s="10">
+        <v>1</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+    </row>
+    <row r="33" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="D33" s="13">
+        <v>2</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G33" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="18"/>
-      <c r="B30" s="10">
+    <row r="34" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="21"/>
+      <c r="B34" s="1">
         <v>2</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D30" s="10">
-        <v>1</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-    </row>
-    <row r="32" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="1">
-        <v>1</v>
-      </c>
-      <c r="C32" s="14" t="s">
+      <c r="C34" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D32" s="13">
+      <c r="D34" s="13">
+        <v>1</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="9" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A35" s="21"/>
+      <c r="B35" s="1">
+        <v>3</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="D35" s="13">
+        <v>1</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="21"/>
+      <c r="B36" s="1">
+        <v>4</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="D36" s="13">
+        <v>1</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="21"/>
+      <c r="B37" s="1">
+        <v>5</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="D37" s="10">
         <v>2</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E37" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="21"/>
+      <c r="B38" s="1">
+        <v>6</v>
+      </c>
+      <c r="C38" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="G32" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="18"/>
-      <c r="B33" s="1">
-        <v>2</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="D33" s="13">
-        <v>1</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="9" customFormat="1" ht="27" x14ac:dyDescent="0.15">
-      <c r="A34" s="18"/>
-      <c r="B34" s="1">
-        <v>3</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="D34" s="13">
-        <v>1</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="18"/>
-      <c r="B35" s="1">
+      <c r="D38" s="13">
         <v>4</v>
       </c>
-      <c r="C35" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="D35" s="13">
-        <v>1</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="18"/>
-      <c r="B36" s="1">
-        <v>5</v>
-      </c>
-      <c r="C36" s="14" t="s">
+      <c r="E38" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="D36" s="10">
-        <v>2</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G36" s="10" t="s">
+      <c r="G38" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="18"/>
-      <c r="B37" s="1">
-        <v>6</v>
-      </c>
-      <c r="C37" s="14" t="s">
+    <row r="39" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="21"/>
+      <c r="B39" s="1">
+        <v>7</v>
+      </c>
+      <c r="C39" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="D37" s="13">
-        <v>4</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G37" s="10" t="s">
+      <c r="D39" s="13">
+        <v>1</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G39" s="10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="18"/>
-      <c r="B38" s="1">
-        <v>7</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="D38" s="13">
-        <v>1</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="18"/>
-      <c r="B39" s="1">
+    <row r="40" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="21"/>
+      <c r="B40" s="1">
         <v>8</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="D39" s="13">
-        <v>2</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="18"/>
-      <c r="B40" s="1">
-        <v>9</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>178</v>
       </c>
       <c r="D40" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G40" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="21"/>
+      <c r="B41" s="1">
+        <v>9</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D41" s="13">
+        <v>1</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="21"/>
+      <c r="B42" s="1">
+        <v>10</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="D42" s="13">
+        <v>1</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G42" s="10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="18"/>
-      <c r="B41" s="1">
-        <v>10</v>
-      </c>
-      <c r="C41" s="14" t="s">
+    <row r="43" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="21"/>
+      <c r="B43" s="1">
+        <v>11</v>
+      </c>
+      <c r="C43" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D41" s="13">
-        <v>1</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G41" s="10" t="s">
+      <c r="D43" s="13">
+        <v>2</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G43" s="10" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="18"/>
-      <c r="B42" s="1">
-        <v>11</v>
-      </c>
-      <c r="C42" s="14" t="s">
+    <row r="44" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="21"/>
+      <c r="B44" s="1">
+        <v>12</v>
+      </c>
+      <c r="C44" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="D42" s="13">
-        <v>2</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G42" s="10" t="s">
+      <c r="D44" s="13">
+        <v>1</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G44" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="18"/>
-      <c r="B43" s="1">
-        <v>12</v>
-      </c>
-      <c r="C43" s="14" t="s">
+    <row r="45" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="21"/>
+      <c r="B45" s="1">
+        <v>13</v>
+      </c>
+      <c r="C45" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="D43" s="13">
-        <v>1</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G43" s="10" t="s">
+      <c r="D45" s="13">
+        <v>1</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G45" s="10" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="18"/>
-      <c r="B44" s="1">
-        <v>13</v>
-      </c>
-      <c r="C44" s="14" t="s">
+    <row r="46" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="21"/>
+      <c r="B46" s="1">
+        <v>14</v>
+      </c>
+      <c r="C46" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="D44" s="13">
-        <v>1</v>
-      </c>
-      <c r="E44" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G44" s="10" t="s">
+      <c r="D46" s="13">
+        <v>1</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G46" s="10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="18"/>
-      <c r="B45" s="1">
-        <v>14</v>
-      </c>
-      <c r="C45" s="14" t="s">
+    <row r="47" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="21"/>
+      <c r="B47" s="1">
+        <v>15</v>
+      </c>
+      <c r="C47" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="D45" s="13">
-        <v>1</v>
-      </c>
-      <c r="E45" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G45" s="10" t="s">
+      <c r="D47" s="13">
+        <v>1</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G47" s="10" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="18"/>
-      <c r="B46" s="1">
-        <v>15</v>
-      </c>
-      <c r="C46" s="14" t="s">
+    <row r="48" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="21"/>
+      <c r="B48" s="1">
+        <v>16</v>
+      </c>
+      <c r="C48" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="D46" s="13">
-        <v>1</v>
-      </c>
-      <c r="E46" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G46" s="10" t="s">
+      <c r="D48" s="13">
+        <v>1</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G48" s="10" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="18"/>
-      <c r="B47" s="1">
-        <v>16</v>
-      </c>
-      <c r="C47" s="14" t="s">
+    <row r="49" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="21"/>
+      <c r="B49" s="1">
+        <v>17</v>
+      </c>
+      <c r="C49" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="D47" s="13">
-        <v>1</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G47" s="10" t="s">
+      <c r="D49" s="13">
+        <v>1</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G49" s="10" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="18"/>
-      <c r="B48" s="1">
-        <v>17</v>
-      </c>
-      <c r="C48" s="14" t="s">
+    <row r="50" spans="1:7" s="9" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A50" s="21"/>
+      <c r="B50" s="10">
+        <v>18</v>
+      </c>
+      <c r="C50" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="D48" s="13">
-        <v>1</v>
-      </c>
-      <c r="E48" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" s="9" customFormat="1" ht="27" x14ac:dyDescent="0.15">
-      <c r="A49" s="18"/>
-      <c r="B49" s="10">
-        <v>18</v>
-      </c>
-      <c r="C49" s="15" t="s">
+      <c r="D50" s="13">
+        <v>1</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="21"/>
+      <c r="B51" s="10">
+        <v>19</v>
+      </c>
+      <c r="C51" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="D49" s="13">
-        <v>1</v>
-      </c>
-      <c r="E49" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G49" s="10" t="s">
+      <c r="D51" s="13">
+        <v>1</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G51" s="10" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="18"/>
-      <c r="B50" s="10">
-        <v>19</v>
-      </c>
-      <c r="C50" s="14" t="s">
+    <row r="52" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="21"/>
+      <c r="B52" s="10">
+        <v>20</v>
+      </c>
+      <c r="C52" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="D50" s="13">
-        <v>1</v>
-      </c>
-      <c r="E50" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G50" s="10" t="s">
+      <c r="D52" s="13">
+        <v>1</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G52" s="10" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="18"/>
-      <c r="B51" s="10">
-        <v>20</v>
-      </c>
-      <c r="C51" s="14" t="s">
+    <row r="53" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="21"/>
+      <c r="B53" s="10">
+        <v>21</v>
+      </c>
+      <c r="C53" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="D51" s="13">
-        <v>1</v>
-      </c>
-      <c r="E51" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G51" s="10" t="s">
+      <c r="D53" s="13">
+        <v>1</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G53" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="18"/>
-      <c r="B52" s="10">
-        <v>21</v>
-      </c>
-      <c r="C52" s="14" t="s">
+    <row r="54" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="21"/>
+      <c r="B54" s="10">
+        <v>22</v>
+      </c>
+      <c r="C54" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="D52" s="13">
-        <v>1</v>
-      </c>
-      <c r="E52" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G52" s="10" t="s">
+      <c r="D54" s="13">
+        <v>1</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G54" s="10" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="18"/>
-      <c r="B53" s="10">
-        <v>22</v>
-      </c>
-      <c r="C53" s="14" t="s">
+    <row r="55" spans="1:7" s="9" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A55" s="21"/>
+      <c r="B55" s="10">
+        <v>23</v>
+      </c>
+      <c r="C55" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="D53" s="13">
-        <v>1</v>
-      </c>
-      <c r="E53" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G53" s="10" t="s">
+      <c r="D55" s="13">
+        <v>1</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G55" s="10" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="9" customFormat="1" ht="27" x14ac:dyDescent="0.15">
-      <c r="A54" s="18"/>
-      <c r="B54" s="10">
-        <v>23</v>
-      </c>
-      <c r="C54" s="11" t="s">
+    <row r="56" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="21"/>
+      <c r="B56" s="10">
+        <v>24</v>
+      </c>
+      <c r="C56" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="D54" s="13">
-        <v>1</v>
-      </c>
-      <c r="E54" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G54" s="10" t="s">
+      <c r="D56" s="13">
+        <v>1</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G56" s="10" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="18"/>
-      <c r="B55" s="10">
-        <v>24</v>
-      </c>
-      <c r="C55" s="14" t="s">
+    <row r="57" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="21"/>
+      <c r="B57" s="10">
+        <v>25</v>
+      </c>
+      <c r="C57" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="D55" s="13">
-        <v>1</v>
-      </c>
-      <c r="E55" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G55" s="10" t="s">
+      <c r="D57" s="13">
+        <v>1</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G57" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="18"/>
-      <c r="B56" s="10">
-        <v>25</v>
-      </c>
-      <c r="C56" s="14" t="s">
+    <row r="58" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="21"/>
+      <c r="B58" s="10">
+        <v>26</v>
+      </c>
+      <c r="C58" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="D56" s="13">
-        <v>1</v>
-      </c>
-      <c r="E56" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G56" s="10" t="s">
+      <c r="D58" s="13">
+        <v>1</v>
+      </c>
+      <c r="E58" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G58" s="10" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="18"/>
-      <c r="B57" s="10">
-        <v>26</v>
-      </c>
-      <c r="C57" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="D57" s="13">
-        <v>1</v>
-      </c>
-      <c r="E57" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G57" s="10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="18"/>
-      <c r="B58" s="10">
+    <row r="59" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="21"/>
+      <c r="B59" s="10">
         <v>27</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="D58" s="10">
-        <v>1</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F58"/>
-      <c r="G58" s="10" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="18"/>
-      <c r="B59" s="10">
-        <v>28</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D59" s="10">
         <v>1</v>
@@ -2327,88 +2400,89 @@
       </c>
       <c r="F59"/>
       <c r="G59" s="10" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A60" s="18"/>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="21"/>
       <c r="B60" s="10">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D60" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="F60"/>
       <c r="G60" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A61" s="18"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="10">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D61" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G61" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A62" s="21"/>
+      <c r="B62" s="10">
+        <v>30</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D62" s="10">
+        <v>1</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A63" s="21"/>
+      <c r="B63" s="10">
+        <v>31</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D63" s="10">
+        <v>2</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G63" s="10" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A62" s="18"/>
-      <c r="B62" s="10">
-        <v>31</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D62" s="10">
-        <v>2</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G62" s="10" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A63" s="18"/>
-      <c r="B63" s="10">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A64" s="21"/>
+      <c r="B64" s="10">
         <v>32</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="D63" s="10">
-        <v>1</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G63" s="10" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A64" s="18"/>
-      <c r="B64" s="10">
-        <v>33</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D64" s="10">
         <v>1</v>
@@ -2417,16 +2491,16 @@
         <v>6</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A65" s="18"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A65" s="21"/>
       <c r="B65" s="10">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D65" s="10">
         <v>1</v>
@@ -2435,16 +2509,16 @@
         <v>6</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="A66" s="18"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A66" s="21"/>
       <c r="B66" s="10">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D66" s="10">
         <v>1</v>
@@ -2452,385 +2526,452 @@
       <c r="E66" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F66" s="11" t="s">
-        <v>143</v>
-      </c>
       <c r="G66" s="10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A67" s="18"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="27" x14ac:dyDescent="0.15">
+      <c r="A67" s="21"/>
       <c r="B67" s="10">
+        <v>35</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D67" s="10">
+        <v>1</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A68" s="21"/>
+      <c r="B68" s="10">
         <v>36</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D67" s="10">
-        <v>1</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G67" s="10" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A68" s="18"/>
-      <c r="B68" s="10">
-        <v>37</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="D68" s="10">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A69" s="18"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A69" s="21"/>
       <c r="B69" s="10">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D69" s="10">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F69" t="s">
+      <c r="G69" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A70" s="21"/>
+      <c r="B70" s="10">
+        <v>38</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D70" s="10">
+        <v>1</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F70" t="s">
         <v>55</v>
       </c>
-      <c r="G69" s="10" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A70" s="17"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
-      <c r="D70" s="17"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="17"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A71" s="18" t="s">
+      <c r="G70" s="10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A71" s="20"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="20"/>
+      <c r="F71" s="20"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A72" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B71" s="1">
-        <v>1</v>
-      </c>
-      <c r="C71" s="2" t="s">
+      <c r="B72" s="1">
+        <v>1</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D71" s="10">
+      <c r="D72" s="10">
         <v>3</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F71" t="s">
-        <v>86</v>
-      </c>
-      <c r="G71" s="10" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A72" s="18"/>
-      <c r="B72" s="1">
-        <v>2</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D72" s="10">
-        <v>1</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="F72" t="s">
+        <v>85</v>
+      </c>
       <c r="G72" s="10" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A73" s="21"/>
+      <c r="B73" s="1">
+        <v>2</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D73" s="10">
+        <v>1</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G73" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A74" s="20"/>
+      <c r="B74" s="20"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="20"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A75" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B75" s="1">
+        <v>1</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D75" s="10">
+        <v>1</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F75" t="s">
+        <v>68</v>
+      </c>
+      <c r="G75" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A73" s="17"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="17"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A74" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B74" s="1">
-        <v>1</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D74" s="10">
-        <v>1</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F74" t="s">
-        <v>68</v>
-      </c>
-      <c r="G74" s="10" t="s">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A76" s="21"/>
+      <c r="B76" s="1">
+        <v>2</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D76" s="10">
+        <v>1</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F76" t="s">
+        <v>71</v>
+      </c>
+      <c r="G76" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A75" s="18"/>
-      <c r="B75" s="1">
-        <v>2</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D75" s="10">
-        <v>1</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F75" t="s">
-        <v>71</v>
-      </c>
-      <c r="G75" s="10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A76" s="18"/>
-      <c r="B76" s="1">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A77" s="21"/>
+      <c r="B77" s="1">
         <v>3</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D76" s="10">
-        <v>1</v>
-      </c>
-      <c r="E76" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G76" s="10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="18"/>
-      <c r="B77" s="1">
-        <v>4</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D77" s="8">
+      <c r="D77" s="10">
         <v>1</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G77" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="21"/>
+      <c r="B78" s="1">
+        <v>4</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D78" s="8">
+        <v>1</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G78" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A79" s="21"/>
+      <c r="B79" s="1">
+        <v>5</v>
+      </c>
+      <c r="C79" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D79" s="10">
+        <v>3</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G79" s="10" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A78" s="18"/>
-      <c r="B78" s="1">
-        <v>5</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D78" s="10">
-        <v>2</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G78" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A79" s="18"/>
-      <c r="B79" s="1">
+      <c r="H79" s="8" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="27" x14ac:dyDescent="0.15">
+      <c r="A80" s="21"/>
+      <c r="B80" s="1">
         <v>6</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C80" s="22" t="s">
         <v>76</v>
-      </c>
-      <c r="D79" s="10">
-        <v>1</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G79" s="10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A80" s="18"/>
-      <c r="B80" s="1">
-        <v>7</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="D80" s="10">
         <v>2</v>
       </c>
       <c r="E80" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G80" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="H80" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A81" s="21"/>
+      <c r="B81" s="1">
+        <v>7</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D81" s="10">
+        <v>2</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G81" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A82" s="21"/>
+      <c r="B82" s="1">
+        <v>8</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G80" s="10" t="s">
+      <c r="D82" s="10">
+        <v>1</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F82" t="s">
+        <v>81</v>
+      </c>
+      <c r="G82" s="10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A81" s="18"/>
-      <c r="B81" s="1">
-        <v>8</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D81" s="10">
-        <v>1</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F81" t="s">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A83" s="21"/>
+      <c r="B83" s="1">
+        <v>9</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G81" s="10" t="s">
+      <c r="D83" s="10">
+        <v>2</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F83" t="s">
+        <v>83</v>
+      </c>
+      <c r="G83" s="10" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A82" s="18"/>
-      <c r="B82" s="1">
-        <v>9</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D82" s="10">
-        <v>2</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F82" t="s">
+    <row r="84" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="21"/>
+      <c r="B84" s="4">
+        <v>10</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G82" s="10" t="s">
+      <c r="D84" s="10">
+        <v>1</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F84" s="5"/>
+      <c r="G84" s="10" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="18"/>
-      <c r="B83" s="4">
-        <v>10</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D83" s="10">
-        <v>1</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G83" s="10" t="s">
+    <row r="85" spans="1:8" s="17" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A85" s="21"/>
+      <c r="B85" s="18">
+        <v>11</v>
+      </c>
+      <c r="C85" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="D85" s="18">
+        <v>1</v>
+      </c>
+      <c r="E85" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="G85" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="H85" s="8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A86" s="21"/>
+      <c r="B86" s="18">
+        <v>12</v>
+      </c>
+      <c r="C86" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="D86" s="18">
+        <v>1</v>
+      </c>
+      <c r="E86" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="G86" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="H86" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A87" s="20"/>
+      <c r="B87" s="20"/>
+      <c r="C87" s="20"/>
+      <c r="D87" s="20"/>
+      <c r="E87" s="20"/>
+      <c r="F87" s="20"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A88" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B88" s="1">
+        <v>1</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D88" s="10">
+        <v>6</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G88" s="10" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A84" s="17"/>
-      <c r="B84" s="17"/>
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="17"/>
-      <c r="F84" s="17"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A85" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B85" s="1">
-        <v>1</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D85" s="10">
-        <v>6</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G85" s="10" t="s">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A89" s="21"/>
+      <c r="B89" s="1">
+        <v>3</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D89" s="10">
+        <v>1</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G89" s="10" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A86" s="18"/>
-      <c r="B86" s="1">
-        <v>3</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D86" s="10">
-        <v>1</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G86" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A71:F71"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="A75:A86"/>
+    <mergeCell ref="A33:A70"/>
     <mergeCell ref="H1:Z1"/>
-    <mergeCell ref="A73:F73"/>
+    <mergeCell ref="A74:F74"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A21:A27"/>
-    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A29:F29"/>
     <mergeCell ref="A5:A19"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A84:F84"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="A74:A83"/>
-    <mergeCell ref="A32:A69"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A21:A28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>